<commit_message>
Getting contest data through helper function
</commit_message>
<xml_diff>
--- a/contest_data.xlsx
+++ b/contest_data.xlsx
@@ -441,8 +441,8 @@
   </sheetPr>
   <dimension ref="A1:D70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D70"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -451,8 +451,8 @@
     <col width="9.140625" customWidth="1" style="1" min="2" max="2"/>
     <col width="10.140625" bestFit="1" customWidth="1" style="1" min="3" max="3"/>
     <col width="22.7109375" bestFit="1" customWidth="1" style="1" min="4" max="4"/>
-    <col width="9.140625" customWidth="1" style="1" min="5" max="8"/>
-    <col width="9.140625" customWidth="1" style="1" min="9" max="16384"/>
+    <col width="9.140625" customWidth="1" style="1" min="5" max="9"/>
+    <col width="9.140625" customWidth="1" style="1" min="10" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -505,7 +505,7 @@
         <v>1957</v>
       </c>
       <c r="C3" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
@@ -523,7 +523,7 @@
         <v>1958</v>
       </c>
       <c r="C4" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
@@ -541,7 +541,7 @@
         <v>1959</v>
       </c>
       <c r="C5" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="1" t="inlineStr">
         <is>
@@ -559,7 +559,7 @@
         <v>1960</v>
       </c>
       <c r="C6" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1" t="inlineStr">
         <is>
@@ -577,7 +577,7 @@
         <v>1961</v>
       </c>
       <c r="C7" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1" t="inlineStr">
         <is>
@@ -595,7 +595,7 @@
         <v>1962</v>
       </c>
       <c r="C8" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="1" t="inlineStr">
         <is>
@@ -613,7 +613,7 @@
         <v>1963</v>
       </c>
       <c r="C9" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="1" t="inlineStr">
         <is>
@@ -631,7 +631,7 @@
         <v>1964</v>
       </c>
       <c r="C10" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="1" t="inlineStr">
         <is>
@@ -649,7 +649,7 @@
         <v>1965</v>
       </c>
       <c r="C11" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="1" t="inlineStr">
         <is>
@@ -667,7 +667,7 @@
         <v>1966</v>
       </c>
       <c r="C12" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="1" t="inlineStr">
         <is>
@@ -685,7 +685,7 @@
         <v>1967</v>
       </c>
       <c r="C13" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="1" t="inlineStr">
         <is>
@@ -703,7 +703,7 @@
         <v>1968</v>
       </c>
       <c r="C14" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="1" t="inlineStr">
         <is>
@@ -721,7 +721,7 @@
         <v>1969</v>
       </c>
       <c r="C15" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="1" t="inlineStr">
         <is>
@@ -739,7 +739,7 @@
         <v>1970</v>
       </c>
       <c r="C16" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="1" t="inlineStr">
         <is>
@@ -757,7 +757,7 @@
         <v>1971</v>
       </c>
       <c r="C17" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="1" t="inlineStr">
         <is>
@@ -775,7 +775,7 @@
         <v>1972</v>
       </c>
       <c r="C18" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="1" t="inlineStr">
         <is>
@@ -793,7 +793,7 @@
         <v>1973</v>
       </c>
       <c r="C19" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="1" t="inlineStr">
         <is>
@@ -811,7 +811,7 @@
         <v>1974</v>
       </c>
       <c r="C20" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="1" t="inlineStr">
         <is>
@@ -829,7 +829,7 @@
         <v>1975</v>
       </c>
       <c r="C21" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="1" t="inlineStr">
         <is>
@@ -847,7 +847,7 @@
         <v>1976</v>
       </c>
       <c r="C22" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="1" t="inlineStr">
         <is>
@@ -865,7 +865,7 @@
         <v>1977</v>
       </c>
       <c r="C23" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="1" t="inlineStr">
         <is>
@@ -883,7 +883,7 @@
         <v>1978</v>
       </c>
       <c r="C24" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="1" t="inlineStr">
         <is>
@@ -901,7 +901,7 @@
         <v>1979</v>
       </c>
       <c r="C25" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="1" t="inlineStr">
         <is>
@@ -919,7 +919,7 @@
         <v>1980</v>
       </c>
       <c r="C26" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26" s="1" t="inlineStr">
         <is>
@@ -937,7 +937,7 @@
         <v>1981</v>
       </c>
       <c r="C27" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" s="1" t="inlineStr">
         <is>
@@ -955,7 +955,7 @@
         <v>1982</v>
       </c>
       <c r="C28" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" s="1" t="inlineStr">
         <is>
@@ -973,7 +973,7 @@
         <v>1983</v>
       </c>
       <c r="C29" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D29" s="1" t="inlineStr">
         <is>
@@ -991,7 +991,7 @@
         <v>1984</v>
       </c>
       <c r="C30" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30" s="1" t="inlineStr">
         <is>
@@ -1009,7 +1009,7 @@
         <v>1985</v>
       </c>
       <c r="C31" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31" s="1" t="inlineStr">
         <is>
@@ -1027,7 +1027,7 @@
         <v>1986</v>
       </c>
       <c r="C32" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D32" s="1" t="inlineStr">
         <is>
@@ -1045,7 +1045,7 @@
         <v>1987</v>
       </c>
       <c r="C33" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D33" s="1" t="inlineStr">
         <is>
@@ -1063,7 +1063,7 @@
         <v>1988</v>
       </c>
       <c r="C34" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" s="1" t="inlineStr">
         <is>
@@ -1081,7 +1081,7 @@
         <v>1989</v>
       </c>
       <c r="C35" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D35" s="1" t="inlineStr">
         <is>
@@ -1099,7 +1099,7 @@
         <v>1990</v>
       </c>
       <c r="C36" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D36" s="1" t="inlineStr">
         <is>
@@ -1117,7 +1117,7 @@
         <v>1991</v>
       </c>
       <c r="C37" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37" s="1" t="inlineStr">
         <is>
@@ -1135,7 +1135,7 @@
         <v>1992</v>
       </c>
       <c r="C38" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D38" s="1" t="inlineStr">
         <is>
@@ -1153,7 +1153,7 @@
         <v>1993</v>
       </c>
       <c r="C39" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39" s="1" t="inlineStr">
         <is>
@@ -1171,7 +1171,7 @@
         <v>1994</v>
       </c>
       <c r="C40" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40" s="1" t="inlineStr">
         <is>
@@ -1189,7 +1189,7 @@
         <v>1995</v>
       </c>
       <c r="C41" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D41" s="1" t="inlineStr">
         <is>
@@ -1207,7 +1207,7 @@
         <v>1996</v>
       </c>
       <c r="C42" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42" s="1" t="inlineStr">
         <is>
@@ -1225,7 +1225,7 @@
         <v>1997</v>
       </c>
       <c r="C43" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D43" s="1" t="inlineStr">
         <is>
@@ -1243,7 +1243,7 @@
         <v>1998</v>
       </c>
       <c r="C44" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D44" s="1" t="inlineStr">
         <is>
@@ -1261,7 +1261,7 @@
         <v>1999</v>
       </c>
       <c r="C45" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D45" s="1" t="inlineStr">
         <is>
@@ -1279,7 +1279,7 @@
         <v>2000</v>
       </c>
       <c r="C46" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D46" s="1" t="inlineStr">
         <is>
@@ -1297,7 +1297,7 @@
         <v>2001</v>
       </c>
       <c r="C47" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D47" s="1" t="inlineStr">
         <is>
@@ -1315,7 +1315,7 @@
         <v>2002</v>
       </c>
       <c r="C48" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D48" s="1" t="inlineStr">
         <is>
@@ -1333,7 +1333,7 @@
         <v>2003</v>
       </c>
       <c r="C49" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49" s="1" t="inlineStr">
         <is>
@@ -1351,7 +1351,7 @@
         <v>2004</v>
       </c>
       <c r="C50" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D50" s="1" t="inlineStr">
         <is>
@@ -1369,7 +1369,7 @@
         <v>2005</v>
       </c>
       <c r="C51" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D51" s="1" t="inlineStr">
         <is>
@@ -1387,7 +1387,7 @@
         <v>2006</v>
       </c>
       <c r="C52" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D52" s="1" t="inlineStr">
         <is>
@@ -1405,7 +1405,7 @@
         <v>2007</v>
       </c>
       <c r="C53" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53" s="1" t="inlineStr">
         <is>
@@ -1423,7 +1423,7 @@
         <v>2008</v>
       </c>
       <c r="C54" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D54" s="1" t="inlineStr">
         <is>
@@ -1441,7 +1441,7 @@
         <v>2009</v>
       </c>
       <c r="C55" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D55" s="1" t="inlineStr">
         <is>
@@ -1459,7 +1459,7 @@
         <v>2010</v>
       </c>
       <c r="C56" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D56" s="1" t="inlineStr">
         <is>
@@ -1477,7 +1477,7 @@
         <v>2011</v>
       </c>
       <c r="C57" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D57" s="1" t="inlineStr">
         <is>
@@ -1495,7 +1495,7 @@
         <v>2012</v>
       </c>
       <c r="C58" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D58" s="1" t="inlineStr">
         <is>
@@ -1513,7 +1513,7 @@
         <v>2013</v>
       </c>
       <c r="C59" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D59" s="1" t="inlineStr">
         <is>
@@ -1531,7 +1531,7 @@
         <v>2014</v>
       </c>
       <c r="C60" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D60" s="1" t="inlineStr">
         <is>
@@ -1549,7 +1549,7 @@
         <v>2015</v>
       </c>
       <c r="C61" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D61" s="1" t="inlineStr">
         <is>
@@ -1567,7 +1567,7 @@
         <v>2016</v>
       </c>
       <c r="C62" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D62" s="1" t="inlineStr">
         <is>
@@ -1585,7 +1585,7 @@
         <v>2017</v>
       </c>
       <c r="C63" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D63" s="1" t="inlineStr">
         <is>
@@ -1603,7 +1603,7 @@
         <v>2018</v>
       </c>
       <c r="C64" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D64" s="1" t="inlineStr">
         <is>
@@ -1621,7 +1621,7 @@
         <v>2019</v>
       </c>
       <c r="C65" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D65" s="1" t="inlineStr">
         <is>
@@ -1639,7 +1639,7 @@
         <v>2020</v>
       </c>
       <c r="C66" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D66" s="1" t="inlineStr">
         <is>
@@ -1657,7 +1657,7 @@
         <v>2021</v>
       </c>
       <c r="C67" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D67" s="1" t="inlineStr">
         <is>
@@ -1675,7 +1675,7 @@
         <v>2022</v>
       </c>
       <c r="C68" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D68" s="1" t="inlineStr">
         <is>
@@ -1693,7 +1693,7 @@
         <v>2023</v>
       </c>
       <c r="C69" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D69" s="1" t="inlineStr">
         <is>
@@ -1711,7 +1711,7 @@
         <v>2024</v>
       </c>
       <c r="C70" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D70" s="1" t="inlineStr">
         <is>

</xml_diff>